<commit_message>
chatgpt4.0: renamed project name accordingly
</commit_message>
<xml_diff>
--- a/prompts.xlsx
+++ b/prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDE549-AD16-4BA8-9A0F-6F040EB02B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20604712-3E4E-4915-8E30-23B5AFCB8366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Neuentwicklung</t>
   </si>
@@ -47,17 +47,50 @@
     <t>Ergänzte Zeilen</t>
   </si>
   <si>
-    <t>Prompt #1</t>
-  </si>
-  <si>
-    <t>Initial Prompt</t>
+    <t>Initial Prompt #1</t>
+  </si>
+  <si>
+    <t>Prompt #2</t>
+  </si>
+  <si>
+    <t>REQ#1</t>
+  </si>
+  <si>
+    <t>Prompt #3</t>
+  </si>
+  <si>
+    <t>REQ#2 + 2a</t>
+  </si>
+  <si>
+    <t>Prompt #4</t>
+  </si>
+  <si>
+    <t>REQ #2b + 2c</t>
+  </si>
+  <si>
+    <t>REQ #3 + 3a</t>
+  </si>
+  <si>
+    <t>Prompt #5</t>
+  </si>
+  <si>
+    <t>REQ #4 +4a + 4b</t>
+  </si>
+  <si>
+    <t>Prompt #6</t>
+  </si>
+  <si>
+    <t>REQ #4c + 4d</t>
+  </si>
+  <si>
+    <t>Prompt #7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,13 +105,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,9 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -376,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -406,24 +454,134 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
chatgpt3.5: screenshots and coverage
</commit_message>
<xml_diff>
--- a/prompts.xlsx
+++ b/prompts.xlsx
@@ -8,29 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED2D2F9-0D87-4F6D-9CE4-9E8E5BCABE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529999F4-7FD3-44E0-8DEA-6B120E6C704D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChatGPT4.0" sheetId="1" r:id="rId1"/>
     <sheet name="ChatGPT3.5" sheetId="2" r:id="rId2"/>
     <sheet name="Gemini" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>Neuentwicklung</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>Anzahl Prompts</t>
   </si>
@@ -107,22 +115,46 @@
     <t>95.3%</t>
   </si>
   <si>
-    <t>Branches</t>
-  </si>
-  <si>
-    <t>Functions</t>
-  </si>
-  <si>
     <t>101/106</t>
   </si>
   <si>
-    <t>function coverage</t>
-  </si>
-  <si>
     <t>source code total lines</t>
   </si>
   <si>
     <t>total lines</t>
+  </si>
+  <si>
+    <t>Sum (Tests)</t>
+  </si>
+  <si>
+    <t>Sum (REQ)</t>
+  </si>
+  <si>
+    <t>Sum (All)</t>
+  </si>
+  <si>
+    <t>total source code lines written by AI (rough)</t>
+  </si>
+  <si>
+    <t>* Assuming the delta did no overwrite changes already made</t>
+  </si>
+  <si>
+    <t>Vorgenommene Änderungen / Anzahl gesamte Source Code lines</t>
+  </si>
+  <si>
+    <t>Neuentwicklung 4.0</t>
+  </si>
+  <si>
+    <t>Neuentwicklung 3.5</t>
+  </si>
+  <si>
+    <t>Vorgenommene Änderungen (Bereinigte Additionen) / Anzahl gesamte Source Code lines</t>
+  </si>
+  <si>
+    <t>* assuming same code format as with gpt4.0</t>
+  </si>
+  <si>
+    <t>102/123</t>
   </si>
 </sst>
 </file>
@@ -153,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,12 +217,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -465,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,39 +521,39 @@
     <col min="6" max="6" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -524,212 +564,285 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="G5" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <f>SUM(D5:D20)</f>
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E5:E20)</f>
         <v>9</v>
       </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="F21">
+        <f>SUM(F17:F20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="E25">
+        <v>14</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18">
-        <v>13</v>
-      </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-      <c r="E19">
-        <v>14</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="E26">
+        <v>62</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="D20">
-        <v>13</v>
-      </c>
-      <c r="E20">
-        <v>62</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>22</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28">
+        <f>SUM(D24:D27)</f>
+        <v>45</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E24:E27)</f>
+        <v>108</v>
+      </c>
+      <c r="F28">
+        <f>SUM(F24:F27)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <v>45395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <f>SUM(D21,D28)</f>
+        <v>51</v>
+      </c>
+      <c r="E30">
+        <f>SUM(E21,E28)</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="D21">
-        <v>5</v>
-      </c>
-      <c r="E21">
-        <v>22</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="B39">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="4">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B40">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="4">
-        <v>519</v>
+      <c r="B42" s="5">
+        <f>(B39- (E30-D30))/B39</f>
+        <v>0.85067873303167418</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -740,12 +853,340 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B69EF8-1CC8-45E9-9F24-14F0DE26F736}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>45396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>45397</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <f>SUM(D5:D20)</f>
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E5:E20)</f>
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <f>SUM(F17:F20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>17</v>
+      </c>
+      <c r="G27" s="6">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28">
+        <f>SUM(D24:D27)</f>
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E24:E27)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <f>SUM(D21,D28)</f>
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <f>SUM(E21,E28)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="5">
+        <f>(B39- (E30-D30))/B39</f>
+        <v>0.92233009708737868</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
all: using ../analysis_defaults from flutter itself for flutter analyze now
</commit_message>
<xml_diff>
--- a/prompts.xlsx
+++ b/prompts.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41EDA97-BEF8-4C31-96D3-A777074F5986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31A90A6-4D70-4882-B05A-C79AFCC05A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChatGPT4.0" sheetId="1" r:id="rId1"/>
     <sheet name="ChatGPT3.5" sheetId="2" r:id="rId2"/>
     <sheet name="Gemini" sheetId="4" r:id="rId3"/>
-    <sheet name="Muster" sheetId="6" r:id="rId4"/>
+    <sheet name="Vergleich" sheetId="7" r:id="rId4"/>
+    <sheet name="Muster" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t>Anzahl Prompts</t>
   </si>
@@ -235,36 +236,6 @@
     <t>chatgpt3.5</t>
   </si>
   <si>
-    <t>fehler 1: overflow ansatz</t>
-  </si>
-  <si>
-    <t>fehler 1: overflow komplettlösung</t>
-  </si>
-  <si>
-    <t>fehler 2: unbound ansatz</t>
-  </si>
-  <si>
-    <t>fehler 2: unbound komplettlösung</t>
-  </si>
-  <si>
-    <t>fehler 3: pumpAndSettle</t>
-  </si>
-  <si>
-    <t>fehler 3: pumpAndSettle komplettlösung</t>
-  </si>
-  <si>
-    <t>fehler 4: state komplettlösung</t>
-  </si>
-  <si>
-    <t>fehler 4: state ansatz</t>
-  </si>
-  <si>
-    <t>Summe ansatz</t>
-  </si>
-  <si>
-    <t>Sume Komplettlösung</t>
-  </si>
-  <si>
     <t>Summe: Total</t>
   </si>
   <si>
@@ -274,17 +245,50 @@
     <t xml:space="preserve">Prozent </t>
   </si>
   <si>
-    <t>% Ansatz</t>
-  </si>
-  <si>
-    <t>% Komplettlösung</t>
+    <t>Fehler 1, Overflow</t>
+  </si>
+  <si>
+    <t>Richtiger Ansatz</t>
+  </si>
+  <si>
+    <t>Einsatzfertige Lösung</t>
+  </si>
+  <si>
+    <t>Fehler 2, Unbounded Height</t>
+  </si>
+  <si>
+    <t>Fehler 3, Fehlendes pumpAndSettle</t>
+  </si>
+  <si>
+    <t>Fehler 4, Falsches State-Management</t>
+  </si>
+  <si>
+    <t>Summe: Richtiger Ansatz</t>
+  </si>
+  <si>
+    <t>Rate: Richtiger Ansatz</t>
+  </si>
+  <si>
+    <t>Summe: Einsatzfertige Lösung</t>
+  </si>
+  <si>
+    <t>Rate: Einsatzfertige Lösung</t>
+  </si>
+  <si>
+    <t>* removal of the example test does not count</t>
+  </si>
+  <si>
+    <t>https://github.com/JosipDomazetDev/Bachelorarbeit/commit/b1b2cbdcb4c18e5ece2bec3ba65026ee652487ca</t>
+  </si>
+  <si>
+    <t>fix for web</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +359,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -396,7 +409,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -415,6 +428,7 @@
     <xf numFmtId="16" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -697,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -819,7 +833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -833,12 +847,12 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -852,7 +866,7 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
         <v>28</v>
       </c>
@@ -865,12 +879,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -890,7 +904,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -904,7 +918,7 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -912,13 +926,22 @@
         <v>13</v>
       </c>
       <c r="E26">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G26" s="6">
         <v>45395</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="H26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -932,7 +955,7 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
@@ -942,13 +965,13 @@
       </c>
       <c r="E28">
         <f>SUM(E24:E27)</f>
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G28" s="6">
         <v>45395</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
@@ -958,7 +981,7 @@
       </c>
       <c r="E30">
         <f>SUM(E21,E28)</f>
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -977,7 +1000,7 @@
         <v>25</v>
       </c>
       <c r="B39">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -985,7 +1008,7 @@
         <v>26</v>
       </c>
       <c r="B40">
-        <v>517</v>
+        <v>523</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1008,7 +1031,7 @@
       </c>
       <c r="B47" s="5">
         <f>B45/B40</f>
-        <v>0.49323017408123793</v>
+        <v>0.4875717017208413</v>
       </c>
     </row>
   </sheetData>
@@ -1024,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B69EF8-1CC8-45E9-9F24-14F0DE26F736}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1335,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AA9F7F-CCCD-4A18-AC44-E37887011679}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1626,7 +1649,7 @@
         <v>25</v>
       </c>
       <c r="B39">
-        <v>336</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1634,7 +1657,7 @@
         <v>26</v>
       </c>
       <c r="B40">
-        <v>302</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1651,7 +1674,7 @@
       </c>
       <c r="B47" s="5">
         <f>B45/B40</f>
-        <v>0.31456953642384106</v>
+        <v>0.28273809523809523</v>
       </c>
     </row>
   </sheetData>
@@ -1660,11 +1683,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90338545-767D-469E-9E78-E3198A3F531E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE2CAE0-86D2-4144-B657-0F600BDDFEED}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1742,114 +1779,98 @@
         <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F25">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+      <c r="A26" s="14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="11"/>
+      <c r="A28" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
+      <c r="A29" s="11"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
+      <c r="A30" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="11"/>
+      <c r="A31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
+      <c r="A33" s="11"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="11"/>
+      <c r="A34" s="14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1857,10 +1878,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1873,99 +1894,135 @@
       <c r="A37" s="11"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="B38">
-        <f>SUM(B26,B29,B32,B35)</f>
-        <v>4</v>
-      </c>
-      <c r="C38">
-        <f>SUM(C26,C29,C32,C35)</f>
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <f>SUM(D26,D29,D32,D35)</f>
-        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="10">
-        <f xml:space="preserve"> (B38/F25)</f>
-        <v>1</v>
-      </c>
-      <c r="C39" s="10">
-        <f xml:space="preserve"> (C38/F25)</f>
-        <v>0.75</v>
-      </c>
-      <c r="D39" s="10">
-        <f xml:space="preserve"> (D38/F25)</f>
-        <v>0.5</v>
+        <v>62</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="11"/>
+      <c r="A40" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41">
-        <f>SUM(B27,B30,B33,B36)</f>
-        <v>3</v>
-      </c>
-      <c r="C41">
-        <f>SUM(C27,C30,C33,C36)</f>
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <f>SUM(D27,D30,D33,D36)</f>
-        <v>1</v>
-      </c>
+      <c r="A41" s="11"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="10">
-        <f xml:space="preserve"> (B41/F25)</f>
+        <v>67</v>
+      </c>
+      <c r="B42">
+        <f>SUM(B27,B31,B35,B39)</f>
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <f>SUM(C27,C31,C35,C39)</f>
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <f>SUM(D27,D31,D35,D39)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="10">
+        <f xml:space="preserve"> (B42/F25)</f>
+        <v>1</v>
+      </c>
+      <c r="C43" s="10">
+        <f xml:space="preserve"> (C42/F25)</f>
         <v>0.75</v>
       </c>
-      <c r="C42" s="10">
-        <f xml:space="preserve"> (C41/F25)</f>
-        <v>0</v>
-      </c>
-      <c r="D42" s="10">
-        <f xml:space="preserve"> (D41/F25)</f>
+      <c r="D43" s="10">
+        <f xml:space="preserve"> (D42/F25)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="11"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45">
+        <f>SUM(B28,B32,B36,B40)</f>
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f>SUM(C28,C32,C36,C40)</f>
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <f>SUM(D28,D32,D36,D40)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="10">
+        <f xml:space="preserve"> (B45/F25)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C46" s="10">
+        <f xml:space="preserve"> (C45/F25)</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="10">
+        <f xml:space="preserve"> (D45/F25)</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="11"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44">
-        <f>SUM(B38,B41)</f>
+    <row r="47" spans="1:4">
+      <c r="A47" s="11"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48">
+        <f>SUM(B42,B45)</f>
         <v>7</v>
       </c>
-      <c r="C44">
-        <f t="shared" ref="C44:D44" si="0">SUM(C38,C41)</f>
+      <c r="C48">
+        <f t="shared" ref="C48:D48" si="0">SUM(C42,C45)</f>
         <v>3</v>
       </c>
-      <c r="D44">
+      <c r="D48">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>70</v>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all: added project README
</commit_message>
<xml_diff>
--- a/prompts.xlsx
+++ b/prompts.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31A90A6-4D70-4882-B05A-C79AFCC05A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56401BD3-3AB5-4C00-A288-03D7A7A4B55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="9970" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChatGPT4.0" sheetId="1" r:id="rId1"/>
     <sheet name="ChatGPT3.5" sheetId="2" r:id="rId2"/>
     <sheet name="Gemini" sheetId="4" r:id="rId3"/>
-    <sheet name="Vergleich" sheetId="7" r:id="rId4"/>
-    <sheet name="Muster" sheetId="6" r:id="rId5"/>
+    <sheet name="Musterlösung" sheetId="8" r:id="rId4"/>
+    <sheet name="Fehlerexperiment" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Anzahl Prompts</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Amount of total test code lines</t>
   </si>
   <si>
-    <t>anzahl änderungen geminsam / 2 / lines?</t>
-  </si>
-  <si>
     <t>Musterlösung Github</t>
   </si>
   <si>
@@ -239,12 +236,6 @@
     <t>Summe: Total</t>
   </si>
   <si>
-    <t>anzahl fehler:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prozent </t>
-  </si>
-  <si>
     <t>Fehler 1, Overflow</t>
   </si>
   <si>
@@ -282,13 +273,16 @@
   </si>
   <si>
     <t>fix for web</t>
+  </si>
+  <si>
+    <t>Anzahl Fehler:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +362,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -409,7 +411,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -429,6 +431,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -711,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -932,13 +935,13 @@
         <v>45395</v>
       </c>
       <c r="H26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -984,7 +987,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -995,42 +998,39 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B39">
+      <c r="B36">
         <v>445</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B40">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45">
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="9"/>
-      <c r="D46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="5">
-        <f>B45/B40</f>
+      <c r="B42" s="5">
+        <f>B40/B37</f>
         <v>0.4875717017208413</v>
       </c>
     </row>
@@ -1045,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B69EF8-1CC8-45E9-9F24-14F0DE26F736}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1316,36 +1316,36 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B39">
+      <c r="B36">
         <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>361</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B40">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="5">
-        <f>B45/B40</f>
+      <c r="B42" s="5">
+        <f>B40/B37</f>
         <v>0.24653739612188366</v>
       </c>
     </row>
@@ -1356,10 +1356,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AA9F7F-CCCD-4A18-AC44-E37887011679}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1410,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="6">
-        <v>45396</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1429,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="6">
-        <v>45397</v>
+        <v>45398</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>39</v>
@@ -1451,7 +1451,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="6">
-        <v>45397</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>45397</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1489,7 +1489,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="6">
-        <v>45397</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="6">
-        <v>45397</v>
+        <v>45398</v>
       </c>
       <c r="I20" t="s">
         <v>43</v>
@@ -1543,7 +1543,7 @@
         <v>11</v>
       </c>
       <c r="G24" s="6">
-        <v>45397</v>
+        <v>45399</v>
       </c>
       <c r="I24" t="s">
         <v>44</v>
@@ -1560,7 +1560,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="6">
-        <v>45397</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1574,7 +1574,7 @@
         <v>11</v>
       </c>
       <c r="G26" s="6">
-        <v>45397</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1588,7 +1588,7 @@
         <v>21</v>
       </c>
       <c r="G27" s="6">
-        <v>45397</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1644,36 +1644,36 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B39">
+      <c r="B36">
         <v>302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B40">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="5">
-        <f>B45/B40</f>
+      <c r="B42" s="5">
+        <f>B40/B37</f>
         <v>0.28273809523809523</v>
       </c>
     </row>
@@ -1683,25 +1683,78 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90338545-767D-469E-9E78-E3198A3F531E}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A190455C-7B81-44B2-BE59-A7EC9179E53A}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="23.5">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5">
+        <f>B10/B7</f>
+        <v>0.26956521739130435</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE2CAE0-86D2-4144-B657-0F600BDDFEED}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1714,315 +1767,256 @@
     <col min="6" max="6" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.5">
-      <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="1" spans="1:7" ht="21">
+      <c r="B1" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>26</v>
+      <c r="C1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="11"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="B15">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="5">
-        <f>B20/B15</f>
-        <v>0.26956521739130435</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="21">
-      <c r="B25" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B3,B7,B11,B15)</f>
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C3,C7,C11,C15)</f>
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <f>SUM(D3,D7,D11,D15)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="10">
+        <f xml:space="preserve"> (B18/G1)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="10">
+        <f xml:space="preserve"> (C18/G1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="D19" s="10">
+        <f xml:space="preserve"> (D18/G1)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21">
+        <f>SUM(B4,B8,B12,B16)</f>
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f>SUM(C4,C8,C12,C16)</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>SUM(D4,D8,D12,D16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="10">
+        <f xml:space="preserve"> (B21/G1)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C22" s="10">
+        <f xml:space="preserve"> (C21/G1)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <f xml:space="preserve"> (D21/G1)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="11"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="11"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="11"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="11"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="11"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42">
-        <f>SUM(B27,B31,B35,B39)</f>
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <f>SUM(C27,C31,C35,C39)</f>
+      <c r="B24">
+        <f>SUM(B18,B21)</f>
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:D24" si="0">SUM(C18,C21)</f>
         <v>3</v>
       </c>
-      <c r="D42">
-        <f>SUM(D27,D31,D35,D39)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="10">
-        <f xml:space="preserve"> (B42/F25)</f>
-        <v>1</v>
-      </c>
-      <c r="C43" s="10">
-        <f xml:space="preserve"> (C42/F25)</f>
-        <v>0.75</v>
-      </c>
-      <c r="D43" s="10">
-        <f xml:space="preserve"> (D42/F25)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="11"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45">
-        <f>SUM(B28,B32,B36,B40)</f>
-        <v>3</v>
-      </c>
-      <c r="C45">
-        <f>SUM(C28,C32,C36,C40)</f>
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <f>SUM(D28,D32,D36,D40)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="10">
-        <f xml:space="preserve"> (B45/F25)</f>
-        <v>0.75</v>
-      </c>
-      <c r="C46" s="10">
-        <f xml:space="preserve"> (C45/F25)</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="10">
-        <f xml:space="preserve"> (D45/F25)</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="11"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48">
-        <f>SUM(B42,B45)</f>
-        <v>7</v>
-      </c>
-      <c r="C48">
-        <f t="shared" ref="C48:D48" si="0">SUM(C42,C45)</f>
-        <v>3</v>
-      </c>
-      <c r="D48">
+      <c r="D24">
         <f t="shared" si="0"/>
         <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>